<commit_message>
fixed typo in TestModeKey.xlsx
</commit_message>
<xml_diff>
--- a/excel/TestModeKey.xlsx
+++ b/excel/TestModeKey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hakanerdogmus/dev/pysheetgrader-parent/pysheetgrader-bk/pysheetgrader-core/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F5FF4F-E30D-2348-BDFB-7D732A133DE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{715651B7-5CA6-C942-BD8F-F897E83D1DF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="-700" windowWidth="51200" windowHeight="21060" tabRatio="883" firstSheet="1" activeTab="4" xr2:uid="{6E72627C-1CB6-4848-9B50-C1295434D515}"/>
+    <workbookView xWindow="-50540" yWindow="-740" windowWidth="26820" windowHeight="21100" tabRatio="883" firstSheet="1" activeTab="2" xr2:uid="{6E72627C-1CB6-4848-9B50-C1295434D515}"/>
   </bookViews>
   <sheets>
     <sheet name="SheetGradingOrder" sheetId="1" r:id="rId1"/>
@@ -6022,7 +6022,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="401">
   <si>
     <t>Number</t>
   </si>
@@ -7222,6 +7222,9 @@
   </si>
   <si>
     <t xml:space="preserve">Bug fixed: Check the score by removing --test-mode: when two cells have equivalent formulas, score should not double! </t>
+  </si>
+  <si>
+    <t>T-Constant-AltCell-BothMatch-CheckDblScore-ForcedToFAIL</t>
   </si>
 </sst>
 </file>
@@ -9091,8 +9094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71EABA77-C8A8-0247-A6AC-2452B8B329D1}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
@@ -9306,7 +9309,7 @@
         <v>91</v>
       </c>
       <c r="C12" t="s">
-        <v>382</v>
+        <v>400</v>
       </c>
       <c r="D12" t="s">
         <v>60</v>
@@ -10169,7 +10172,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF83535-20BE-CA43-B82B-2F0E1F118D83}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
@@ -11419,8 +11422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B5E91EC-3DFF-1543-8E9D-3526C440EDB3}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27:J29"/>
+    <sheetView zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
@@ -11965,7 +11968,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
add expected grades to checkorder and test output
</commit_message>
<xml_diff>
--- a/excel/TestModeKey.xlsx
+++ b/excel/TestModeKey.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hakanerdogmus/dev/pysheetgrader-parent/pysheetgrader-core-main/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrew/git/pysheetgrader-core/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFEDDB36-C50E-894F-B2C2-7E92C0942870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F7ABE01-0897-9F4E-BE0B-9B004A539666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="34680" windowHeight="14140" tabRatio="883" activeTab="8" xr2:uid="{6E72627C-1CB6-4848-9B50-C1295434D515}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="14140" tabRatio="883" activeTab="2" xr2:uid="{6E72627C-1CB6-4848-9B50-C1295434D515}"/>
   </bookViews>
   <sheets>
     <sheet name="SheetGradingOrder" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <sheet name="Minimum Work_CheckOrder" sheetId="18" r:id="rId16"/>
     <sheet name="Minimum Work" sheetId="19" r:id="rId17"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -3493,6 +3493,87 @@
         </r>
       </text>
     </comment>
+    <comment ref="C29" authorId="0" shapeId="0" xr:uid="{352D8B4A-FD27-D442-B8D7-A9D580069C10}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>rubric:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: relative
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">alt_cells:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> - B30
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> - B31</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -4599,6 +4680,88 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve"> type: check</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C30" authorId="0" shapeId="0" xr:uid="{A69C7DBC-568D-E649-82BE-A8E5C0983CF8}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>rubric:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: check
+ result: D30
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">alt_cells:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> - B31
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> - B32</t>
         </r>
       </text>
     </comment>
@@ -6002,7 +6165,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="409">
   <si>
     <t>Number</t>
   </si>
@@ -7199,6 +7362,36 @@
   </si>
   <si>
     <t>Check17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relative rubric with alt cells - one alt is identical to orig </t>
+  </si>
+  <si>
+    <t>Rel17</t>
+  </si>
+  <si>
+    <t>T-Relative-AltCell-DupeAltCellCorrect</t>
+  </si>
+  <si>
+    <t>Bug: check the score!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check rubric with alt cells - one alt is identical to orig </t>
+  </si>
+  <si>
+    <t>T-Check-AltCell-DuplicateScore</t>
+  </si>
+  <si>
+    <t>Check18</t>
+  </si>
+  <si>
+    <t>C30</t>
+  </si>
+  <si>
+    <t>T-Check-Alt-Double</t>
+  </si>
+  <si>
+    <t>Expected-Score</t>
   </si>
 </sst>
 </file>
@@ -7309,10 +7502,10 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -8604,8 +8797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A103586-2C0E-0748-80AF-98E299C769E5}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView topLeftCell="C4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9066,10 +9259,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71EABA77-C8A8-0247-A6AC-2452B8B329D1}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9079,7 +9272,7 @@
     <col min="5" max="5" width="71.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9098,8 +9291,11 @@
       <c r="F1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>95</v>
       </c>
@@ -9115,8 +9311,11 @@
       <c r="E2" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>96</v>
       </c>
@@ -9132,8 +9331,11 @@
       <c r="E3" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>97</v>
       </c>
@@ -9152,8 +9354,11 @@
       <c r="F4" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>98</v>
       </c>
@@ -9169,8 +9374,11 @@
       <c r="E5" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>99</v>
       </c>
@@ -9186,8 +9394,11 @@
       <c r="E6" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>100</v>
       </c>
@@ -9206,8 +9417,11 @@
       <c r="F7" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>101</v>
       </c>
@@ -9223,8 +9437,11 @@
       <c r="E8" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>102</v>
       </c>
@@ -9240,8 +9457,11 @@
       <c r="E9" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>103</v>
       </c>
@@ -9257,8 +9477,11 @@
       <c r="E10" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>104</v>
       </c>
@@ -9274,8 +9497,11 @@
       <c r="E11" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>105</v>
       </c>
@@ -9286,13 +9512,16 @@
         <v>382</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E12" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>106</v>
       </c>
@@ -9308,8 +9537,11 @@
       <c r="E13" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>107</v>
       </c>
@@ -9325,8 +9557,11 @@
       <c r="E14" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>380</v>
       </c>
@@ -9342,8 +9577,11 @@
       <c r="E15" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>385</v>
       </c>
@@ -9358,6 +9596,9 @@
       </c>
       <c r="E16" t="s">
         <v>386</v>
+      </c>
+      <c r="G16">
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>
@@ -9371,8 +9612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEB70C9E-5A32-AF4F-951C-2DFC686CB197}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView topLeftCell="C27" zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
-      <selection activeCell="K44" sqref="K44"/>
+    <sheetView topLeftCell="A29" zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9380,7 +9621,7 @@
     <col min="1" max="1" width="30.5" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" customWidth="1"/>
     <col min="3" max="3" width="16.83203125" customWidth="1"/>
-    <col min="5" max="5" width="75.1640625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="75.1640625" style="9" customWidth="1"/>
     <col min="6" max="6" width="7" customWidth="1"/>
     <col min="7" max="7" width="39.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -9406,7 +9647,7 @@
         <v>306</v>
       </c>
       <c r="D4" s="2"/>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>6</v>
       </c>
       <c r="F4" t="s">
@@ -9432,7 +9673,7 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="9" t="s">
         <v>252</v>
       </c>
       <c r="F5" t="s">
@@ -9454,7 +9695,7 @@
         <v>2020</v>
       </c>
       <c r="D6" s="2"/>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="9" t="s">
         <v>274</v>
       </c>
       <c r="F6" t="s">
@@ -9480,7 +9721,7 @@
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="9" t="s">
         <v>255</v>
       </c>
       <c r="F7" t="s">
@@ -9506,7 +9747,7 @@
         <v>202</v>
       </c>
       <c r="D8" s="2"/>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="9" t="s">
         <v>257</v>
       </c>
       <c r="F8" t="s">
@@ -9531,7 +9772,7 @@
         <v>202</v>
       </c>
       <c r="D9" s="2"/>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="9" t="s">
         <v>259</v>
       </c>
       <c r="F9" t="s">
@@ -9557,7 +9798,7 @@
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="9" t="s">
         <v>266</v>
       </c>
       <c r="F10" t="s">
@@ -9583,7 +9824,7 @@
         <v>20.2</v>
       </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="9" t="s">
         <v>267</v>
       </c>
       <c r="F11" t="s">
@@ -9609,7 +9850,7 @@
         <v>20.2</v>
       </c>
       <c r="D12" s="2"/>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="9" t="s">
         <v>281</v>
       </c>
       <c r="F12" t="s">
@@ -9635,7 +9876,7 @@
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="9" t="s">
         <v>284</v>
       </c>
       <c r="F13" t="s">
@@ -9658,7 +9899,7 @@
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="9" t="s">
         <v>284</v>
       </c>
       <c r="F14" t="s">
@@ -9681,7 +9922,7 @@
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="9" t="s">
         <v>284</v>
       </c>
       <c r="F15" t="s">
@@ -9704,7 +9945,7 @@
         <v>40.4</v>
       </c>
       <c r="D16" s="2"/>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="9" t="s">
         <v>298</v>
       </c>
       <c r="F16" t="s">
@@ -9735,7 +9976,7 @@
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="9" t="s">
         <v>295</v>
       </c>
       <c r="F18" t="s">
@@ -9770,7 +10011,7 @@
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="9" t="s">
         <v>304</v>
       </c>
       <c r="F20" t="s">
@@ -9796,7 +10037,7 @@
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="9" t="s">
         <v>266</v>
       </c>
       <c r="F21" t="s">
@@ -9822,7 +10063,7 @@
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="9" t="s">
         <v>345</v>
       </c>
       <c r="F22" t="s">
@@ -9847,7 +10088,7 @@
         <v>39370</v>
       </c>
       <c r="D23" s="2"/>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="9" t="s">
         <v>325</v>
       </c>
       <c r="F23" t="s">
@@ -9869,7 +10110,7 @@
         <v>39370.1</v>
       </c>
       <c r="D24" s="2"/>
-      <c r="E24" s="10" t="s">
+      <c r="E24" s="9" t="s">
         <v>348</v>
       </c>
       <c r="F24" t="s">
@@ -9902,7 +10143,7 @@
         <f>B18*40</f>
         <v>40000</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E26" s="9" t="s">
         <v>355</v>
       </c>
       <c r="F26" s="5" t="s">
@@ -9926,7 +10167,7 @@
         <f>B18*45</f>
         <v>45000</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E27" s="9" t="s">
         <v>352</v>
       </c>
       <c r="F27" s="5" t="s">
@@ -9950,7 +10191,7 @@
         <f xml:space="preserve"> B18*39.37</f>
         <v>39370</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E28" s="9" t="s">
         <v>358</v>
       </c>
       <c r="F28" s="5" t="s">
@@ -9983,7 +10224,7 @@
         <f>ROUNDUP(C6/100, 0)</f>
         <v>21</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="E31" s="9" t="s">
         <v>311</v>
       </c>
       <c r="F31" s="5" t="s">
@@ -10028,7 +10269,7 @@
         <f>B34+B35</f>
         <v>30</v>
       </c>
-      <c r="E36" s="10" t="s">
+      <c r="E36" s="9" t="s">
         <v>359</v>
       </c>
       <c r="F36" t="s">
@@ -10049,7 +10290,7 @@
         <f>B34+B35</f>
         <v>30</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="E37" s="9" t="s">
         <v>360</v>
       </c>
       <c r="F37" t="s">
@@ -10070,7 +10311,7 @@
         <f>B34+B35</f>
         <v>30</v>
       </c>
-      <c r="E38" s="10" t="s">
+      <c r="E38" s="9" t="s">
         <v>361</v>
       </c>
       <c r="F38" t="s">
@@ -10118,7 +10359,7 @@
         <f>B34-B35</f>
         <v>-10</v>
       </c>
-      <c r="E42" s="10" t="s">
+      <c r="E42" s="9" t="s">
         <v>366</v>
       </c>
       <c r="F42" t="s">
@@ -10146,7 +10387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF83535-20BE-CA43-B82B-2F0E1F118D83}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -10601,10 +10842,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F753B85-5CB9-481B-8C77-51ACF6917C73}">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="113" zoomScaleNormal="113" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView topLeftCell="A11" zoomScale="113" zoomScaleNormal="113" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10661,7 +10902,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="10" t="s">
         <v>124</v>
       </c>
       <c r="B5">
@@ -10672,7 +10913,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="9"/>
+      <c r="A6" s="10"/>
       <c r="B6">
         <v>5</v>
       </c>
@@ -10681,7 +10922,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="9"/>
+      <c r="A7" s="10"/>
       <c r="B7">
         <v>10</v>
       </c>
@@ -10690,7 +10931,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="9"/>
+      <c r="A8" s="10"/>
       <c r="B8">
         <v>1</v>
       </c>
@@ -10699,7 +10940,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="9"/>
+      <c r="A9" s="10"/>
       <c r="B9">
         <v>6</v>
       </c>
@@ -11090,6 +11331,48 @@
         <v>191</v>
       </c>
       <c r="B28">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>135</v>
+      </c>
+      <c r="C29">
+        <f>SUM(C5:C9)</f>
+        <v>24</v>
+      </c>
+      <c r="E29" t="s">
+        <v>399</v>
+      </c>
+      <c r="F29" t="s">
+        <v>393</v>
+      </c>
+      <c r="G29" t="s">
+        <v>227</v>
+      </c>
+      <c r="H29" t="s">
+        <v>59</v>
+      </c>
+      <c r="I29" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>136</v>
+      </c>
+      <c r="B30">
+        <f>SUM(C5:C9)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>136</v>
+      </c>
+      <c r="B31">
+        <f>SUM(B16:B20)</f>
         <v>24</v>
       </c>
     </row>
@@ -11104,10 +11387,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5C438D0-7759-4CC5-97B1-26C21A13DC4C}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11386,6 +11669,23 @@
         <v>242</v>
       </c>
     </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>400</v>
+      </c>
+      <c r="B18" t="s">
+        <v>393</v>
+      </c>
+      <c r="C18" t="s">
+        <v>401</v>
+      </c>
+      <c r="D18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" t="s">
+        <v>402</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11394,10 +11694,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B5E91EC-3DFF-1543-8E9D-3526C440EDB3}">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27:J29"/>
+    <sheetView zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11457,7 +11757,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="10" t="s">
         <v>124</v>
       </c>
       <c r="B5">
@@ -11468,7 +11768,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="9"/>
+      <c r="A6" s="10"/>
       <c r="B6">
         <v>5</v>
       </c>
@@ -11477,7 +11777,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="9"/>
+      <c r="A7" s="10"/>
       <c r="B7">
         <v>10</v>
       </c>
@@ -11486,7 +11786,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="9"/>
+      <c r="A8" s="10"/>
       <c r="B8">
         <v>1</v>
       </c>
@@ -11495,7 +11795,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="9"/>
+      <c r="A9" s="10"/>
       <c r="B9">
         <v>6</v>
       </c>
@@ -11926,6 +12226,50 @@
       </c>
       <c r="J29" t="s">
         <v>395</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>135</v>
+      </c>
+      <c r="C30">
+        <f>SUM(C5:C9)</f>
+        <v>24</v>
+      </c>
+      <c r="D30">
+        <v>23.5</v>
+      </c>
+      <c r="F30" t="s">
+        <v>403</v>
+      </c>
+      <c r="G30" t="s">
+        <v>406</v>
+      </c>
+      <c r="H30" t="s">
+        <v>404</v>
+      </c>
+      <c r="I30" t="s">
+        <v>59</v>
+      </c>
+      <c r="J30" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>136</v>
+      </c>
+      <c r="B31">
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>136</v>
+      </c>
+      <c r="B32">
+        <f>SUM(C5:C9)</f>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -11939,10 +12283,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05739818-17B0-D842-BB6C-69A1E595FDFD}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12246,6 +12590,23 @@
         <v>395</v>
       </c>
     </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>405</v>
+      </c>
+      <c r="B19" t="s">
+        <v>406</v>
+      </c>
+      <c r="C19" t="s">
+        <v>407</v>
+      </c>
+      <c r="D19" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" t="s">
+        <v>367</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
make changes to key for constants expected scores
</commit_message>
<xml_diff>
--- a/excel/TestModeKey.xlsx
+++ b/excel/TestModeKey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrew/git/pysheetgrader-core/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F7ABE01-0897-9F4E-BE0B-9B004A539666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF6DDD8-D5C7-F046-9295-E07FFE7B5F6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="14140" tabRatio="883" activeTab="2" xr2:uid="{6E72627C-1CB6-4848-9B50-C1295434D515}"/>
   </bookViews>
@@ -6165,7 +6165,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="410">
   <si>
     <t>Number</t>
   </si>
@@ -7310,9 +7310,6 @@
     <t>Const14</t>
   </si>
   <si>
-    <t>Cell should have been graded correct with alt cell - orig cell correct and matches alt cell too! Possible POSSIBLE BUG - test made to fail to force checking double score when orig and alt cell have the same value!</t>
-  </si>
-  <si>
     <t>T-Constant-AltCell-BothMatch-CheckDblScore-FocedToFAIL</t>
   </si>
   <si>
@@ -7392,6 +7389,12 @@
   </si>
   <si>
     <t>Expected-Score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cell should have been graded correct with alt cell - orig cell correct and matches alt cell too! </t>
+  </si>
+  <si>
+    <t>Cell should have been graded correct with alt cell - orig cell correct and matches alt cell too!</t>
   </si>
 </sst>
 </file>
@@ -8797,8 +8800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A103586-2C0E-0748-80AF-98E299C769E5}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView topLeftCell="C12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9137,13 +9140,13 @@
         <v>91</v>
       </c>
       <c r="G17" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I17" t="s">
-        <v>381</v>
+        <v>408</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -9223,7 +9226,7 @@
         <v>59</v>
       </c>
       <c r="I21" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -9235,19 +9238,19 @@
         <v>39370</v>
       </c>
       <c r="E22" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>309</v>
       </c>
       <c r="G22" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="H22" t="s">
         <v>59</v>
       </c>
       <c r="I22" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
   </sheetData>
@@ -9262,7 +9265,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9292,7 +9295,7 @@
         <v>57</v>
       </c>
       <c r="G1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -9509,13 +9512,13 @@
         <v>91</v>
       </c>
       <c r="C12" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D12" t="s">
         <v>59</v>
       </c>
       <c r="E12" t="s">
-        <v>381</v>
+        <v>409</v>
       </c>
       <c r="G12">
         <v>1.5</v>
@@ -9575,7 +9578,7 @@
         <v>59</v>
       </c>
       <c r="E15" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="G15">
         <v>1.5</v>
@@ -9583,19 +9586,19 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>309</v>
       </c>
       <c r="C16" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D16" t="s">
         <v>59</v>
       </c>
       <c r="E16" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="G16">
         <v>1.5</v>
@@ -11287,7 +11290,7 @@
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F26" t="s">
         <v>179</v>
@@ -11311,7 +11314,7 @@
         <v>24</v>
       </c>
       <c r="E27" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F27" t="s">
         <v>194</v>
@@ -11343,10 +11346,10 @@
         <v>24</v>
       </c>
       <c r="E29" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F29" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G29" t="s">
         <v>227</v>
@@ -11671,19 +11674,19 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>399</v>
+      </c>
+      <c r="B18" t="s">
+        <v>392</v>
+      </c>
+      <c r="C18" t="s">
         <v>400</v>
-      </c>
-      <c r="B18" t="s">
-        <v>393</v>
-      </c>
-      <c r="C18" t="s">
-        <v>401</v>
       </c>
       <c r="D18" t="s">
         <v>59</v>
       </c>
       <c r="E18" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
   </sheetData>
@@ -11815,7 +11818,7 @@
         <v>10.4</v>
       </c>
       <c r="F10" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G10" t="s">
         <v>42</v>
@@ -12110,7 +12113,7 @@
         <v>1023</v>
       </c>
       <c r="F24" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G24" t="s">
         <v>174</v>
@@ -12188,13 +12191,13 @@
         <v>194</v>
       </c>
       <c r="H27" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="I27" t="s">
         <v>60</v>
       </c>
       <c r="J27" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
@@ -12213,19 +12216,19 @@
         <v>1</v>
       </c>
       <c r="F29" t="s">
+        <v>391</v>
+      </c>
+      <c r="G29" t="s">
         <v>392</v>
       </c>
-      <c r="G29" t="s">
-        <v>393</v>
-      </c>
       <c r="H29" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="I29" t="s">
         <v>60</v>
       </c>
       <c r="J29" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
@@ -12240,13 +12243,13 @@
         <v>23.5</v>
       </c>
       <c r="F30" t="s">
+        <v>402</v>
+      </c>
+      <c r="G30" t="s">
+        <v>405</v>
+      </c>
+      <c r="H30" t="s">
         <v>403</v>
-      </c>
-      <c r="G30" t="s">
-        <v>406</v>
-      </c>
-      <c r="H30" t="s">
-        <v>404</v>
       </c>
       <c r="I30" t="s">
         <v>59</v>
@@ -12564,41 +12567,41 @@
         <v>194</v>
       </c>
       <c r="C17" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D17" t="s">
         <v>60</v>
       </c>
       <c r="E17" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B18" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C18" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D18" t="s">
         <v>60</v>
       </c>
       <c r="E18" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>404</v>
+      </c>
+      <c r="B19" t="s">
         <v>405</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>406</v>
-      </c>
-      <c r="C19" t="s">
-        <v>407</v>
       </c>
       <c r="D19" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
commit neg test cases
</commit_message>
<xml_diff>
--- a/excel/TestModeKey.xlsx
+++ b/excel/TestModeKey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrew/git/pysheetgrader/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E3C94B-5FAA-4341-85BC-DD44594684E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5F84A1-D8AE-C74E-BEAA-E75DDB18B53D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="14140" tabRatio="883" activeTab="4" xr2:uid="{6E72627C-1CB6-4848-9B50-C1295434D515}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="14140" tabRatio="883" activeTab="1" xr2:uid="{6E72627C-1CB6-4848-9B50-C1295434D515}"/>
   </bookViews>
   <sheets>
     <sheet name="SheetGradingOrder" sheetId="1" r:id="rId1"/>
@@ -1481,7 +1481,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>rubric:</t>
         </r>
@@ -1491,18 +1490,16 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> </t>
         </r>
@@ -1512,7 +1509,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>score: 1</t>
         </r>
@@ -1522,18 +1518,16 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> </t>
         </r>
@@ -1543,7 +1537,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>type: relative</t>
         </r>
@@ -1553,18 +1546,16 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> </t>
         </r>
@@ -1574,7 +1565,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>parse_excel: true</t>
         </r>
@@ -1584,7 +1574,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -1599,7 +1588,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>rubric:</t>
         </r>
@@ -1609,18 +1597,16 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="18"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> score: 1</t>
         </r>
@@ -1630,18 +1616,16 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="18"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> type: relative</t>
         </r>
@@ -1651,18 +1635,16 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="18"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> parse_excel: true</t>
         </r>
@@ -1676,7 +1658,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>rubric:</t>
         </r>
@@ -1686,18 +1667,16 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="18"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> score: 1</t>
         </r>
@@ -1707,18 +1686,16 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="18"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> type: relative</t>
         </r>
@@ -1728,18 +1705,16 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="18"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> parse_excel: true</t>
         </r>
@@ -1907,7 +1882,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>rubric:</t>
         </r>
@@ -1917,18 +1891,16 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="18"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> score: 1</t>
         </r>
@@ -1938,18 +1910,16 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="18"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> type: relative</t>
         </r>
@@ -1959,18 +1929,16 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="18"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> parse_excel: true
 </t>
@@ -1981,7 +1949,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve"> delta: 0.05
 </t>
@@ -1996,7 +1963,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>rubric:</t>
         </r>
@@ -2006,18 +1972,16 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="18"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> score: 1</t>
         </r>
@@ -2027,18 +1991,16 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="18"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> type: relative</t>
         </r>
@@ -2048,18 +2010,16 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="18"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> parse_excel: true</t>
         </r>
@@ -2073,7 +2033,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>rubric:</t>
         </r>
@@ -2083,18 +2042,16 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="18"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> score: 1</t>
         </r>
@@ -2104,18 +2061,16 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="18"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> type: relative</t>
         </r>
@@ -2125,18 +2080,16 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="18"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> parse_excel: true</t>
         </r>
@@ -2304,7 +2257,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>rubric:</t>
         </r>
@@ -2314,18 +2266,16 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="18"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> score: 1</t>
         </r>
@@ -2335,18 +2285,16 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="18"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> type: relative</t>
         </r>
@@ -2356,18 +2304,16 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="18"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> parse_excel: true</t>
         </r>
@@ -2381,7 +2327,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>rubric:</t>
         </r>
@@ -2391,18 +2336,16 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="18"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> score: 1</t>
         </r>
@@ -2412,18 +2355,16 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="18"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> type: relative</t>
         </r>
@@ -2433,18 +2374,16 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="18"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> parse_excel: true</t>
         </r>
@@ -2458,6 +2397,402 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
+          </rPr>
+          <t>rubric:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: relative</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> parse_excel: true</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B46" authorId="0" shapeId="0" xr:uid="{43A0C2DF-B20F-D143-BCE3-FA769F2A384B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>rubric:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>relative</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> parse_excel: true</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B47" authorId="1" shapeId="0" xr:uid="{819B5873-7A68-B04A-A622-1ECA025DC15C}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>rubric:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>score: 1</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>type: relative</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>parse_excel: true</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B48" authorId="1" shapeId="0" xr:uid="{71EBBE38-7DB9-9B46-B1AD-C775BDB6A879}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>rubric:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: relative</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> parse_excel: true</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B49" authorId="1" shapeId="0" xr:uid="{40FA9D86-0549-854A-A56D-0BE6F8BBC62F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>rubric:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: relative</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> parse_excel: true</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B50" authorId="1" shapeId="0" xr:uid="{BC2F58E3-A7BC-A54D-BC36-696F428B7FFF}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>rubric:</t>
@@ -2522,6 +2857,584 @@
             <rFont val="Calibri"/>
             <family val="2"/>
             <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve"> parse_excel: true</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B51" authorId="1" shapeId="0" xr:uid="{40B83FDC-11DD-3143-A500-51BD2C19BC61}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>rubric:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve"> type: relative</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve"> parse_excel: true</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B52" authorId="1" shapeId="0" xr:uid="{C995DDB5-E619-F94A-8A28-B28F9BEFD0FD}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>rubric:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: relative</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> parse_excel: true
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> delta: 0.05
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B53" authorId="1" shapeId="0" xr:uid="{740BCFAB-91CE-374F-A67C-91D373AA228A}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>rubric:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: relative</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> parse_excel: true</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B54" authorId="1" shapeId="0" xr:uid="{9EB17EE4-2F5D-9E49-B8B1-A11B5EBD8860}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>rubric:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: relative</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> parse_excel: true</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B55" authorId="1" shapeId="0" xr:uid="{5D2EAF2E-9AEF-8043-B9BD-19E7E259D85E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>rubric:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: relative</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> parse_excel: true</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B56" authorId="1" shapeId="0" xr:uid="{45224780-F82C-0D4B-9066-95AC59AFCE10}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>rubric:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: relative</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> parse_excel: true</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B57" authorId="1" shapeId="0" xr:uid="{BB21FCB0-B207-024A-B83B-E669A5D5B19A}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>rubric:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: relative</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> parse_excel: true</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B58" authorId="1" shapeId="0" xr:uid="{8F640E8A-DAD6-9747-9DFC-6424DE8F6A10}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>rubric:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: relative</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> parse_excel: true</t>
         </r>
@@ -9182,7 +10095,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1347" uniqueCount="572">
   <si>
     <t>Number</t>
   </si>
@@ -10781,6 +11694,123 @@
   </si>
   <si>
     <t>XL30</t>
+  </si>
+  <si>
+    <t>XL31</t>
+  </si>
+  <si>
+    <t>XL32</t>
+  </si>
+  <si>
+    <t>XL33</t>
+  </si>
+  <si>
+    <t>XL34</t>
+  </si>
+  <si>
+    <t>XL35</t>
+  </si>
+  <si>
+    <t>XL36</t>
+  </si>
+  <si>
+    <t>XL37</t>
+  </si>
+  <si>
+    <t>XL38</t>
+  </si>
+  <si>
+    <t>XL39</t>
+  </si>
+  <si>
+    <t>XL40</t>
+  </si>
+  <si>
+    <t>XL41</t>
+  </si>
+  <si>
+    <t>XL42</t>
+  </si>
+  <si>
+    <t>XL43</t>
+  </si>
+  <si>
+    <t>B46</t>
+  </si>
+  <si>
+    <t>B47</t>
+  </si>
+  <si>
+    <t>B48</t>
+  </si>
+  <si>
+    <t>B49</t>
+  </si>
+  <si>
+    <t>B50</t>
+  </si>
+  <si>
+    <t>B51</t>
+  </si>
+  <si>
+    <t>B52</t>
+  </si>
+  <si>
+    <t>B53</t>
+  </si>
+  <si>
+    <t>B54</t>
+  </si>
+  <si>
+    <t>B55</t>
+  </si>
+  <si>
+    <t>B56</t>
+  </si>
+  <si>
+    <t>B57</t>
+  </si>
+  <si>
+    <t>B58</t>
+  </si>
+  <si>
+    <t>T-Relative-Excel-Length-Bad</t>
+  </si>
+  <si>
+    <t>T-Relative-XL-SQRT-Bad</t>
+  </si>
+  <si>
+    <t>T-Relative-XL-AVG-Bad</t>
+  </si>
+  <si>
+    <t>T-Relative-XL-ROUND-Bad</t>
+  </si>
+  <si>
+    <t>T-Relative-XL-Concat-Bad</t>
+  </si>
+  <si>
+    <t>T-Relative-XL-Ln-Bad</t>
+  </si>
+  <si>
+    <t>T-Relative-XL-STDEV-Bad</t>
+  </si>
+  <si>
+    <t>T-Relative-XL-COUNTIF-Bad</t>
+  </si>
+  <si>
+    <t>T-Relative-XL-IF1-Bad</t>
+  </si>
+  <si>
+    <t>T-Relative-XL-IF2-Bad</t>
+  </si>
+  <si>
+    <t>T-Relative-XL-Ifand-Bad</t>
+  </si>
+  <si>
+    <t>T-Relative-XL-Ifor-Bad</t>
+  </si>
+  <si>
+    <t>T-Relative-XL-Ifnot-Bad</t>
   </si>
 </sst>
 </file>
@@ -10934,10 +11964,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -11450,7 +12480,7 @@
       </c>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="11" t="s">
         <v>124</v>
       </c>
       <c r="B5">
@@ -11461,7 +12491,7 @@
       </c>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="10"/>
+      <c r="A6" s="11"/>
       <c r="B6">
         <v>5</v>
       </c>
@@ -11470,7 +12500,7 @@
       </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="10"/>
+      <c r="A7" s="11"/>
       <c r="B7">
         <v>10</v>
       </c>
@@ -11479,7 +12509,7 @@
       </c>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="10"/>
+      <c r="A8" s="11"/>
       <c r="B8">
         <v>1</v>
       </c>
@@ -11488,7 +12518,7 @@
       </c>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="10"/>
+      <c r="A9" s="11"/>
       <c r="B9">
         <v>6</v>
       </c>
@@ -13219,10 +14249,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CFDFF2D-5588-974C-8962-7185857425AC}">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
@@ -13261,7 +14291,7 @@
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="11" t="s">
         <v>124</v>
       </c>
       <c r="B5">
@@ -13272,7 +14302,7 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="10"/>
+      <c r="A6" s="11"/>
       <c r="B6">
         <v>5</v>
       </c>
@@ -13284,7 +14314,7 @@
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="10"/>
+      <c r="A7" s="11"/>
       <c r="B7">
         <v>10</v>
       </c>
@@ -13293,7 +14323,7 @@
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="10"/>
+      <c r="A8" s="11"/>
       <c r="B8">
         <v>1</v>
       </c>
@@ -13302,7 +14332,7 @@
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="10"/>
+      <c r="A9" s="11"/>
       <c r="B9">
         <v>6</v>
       </c>
@@ -13520,7 +14550,7 @@
       <c r="A33" t="s">
         <v>482</v>
       </c>
-      <c r="B33" s="11">
+      <c r="B33" s="10">
         <f>SQRT(D6)</f>
         <v>2</v>
       </c>
@@ -13629,6 +14659,84 @@
         <v>523</v>
       </c>
       <c r="B45">
+        <f>IF(NOT(2&lt;1), 0, 100)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="B46" t="b">
+        <f>C21 &gt; LEN("ABCD") - 4 + 10</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="B47" s="10">
+        <f>SQRT(D20)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="B48">
+        <f>AVERAGE(B19:B20)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2">
+      <c r="B49">
+        <f>ROUND(3.5, 0)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2">
+      <c r="B50" t="str">
+        <f>CONCATENATE("4", "", "5")</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2">
+      <c r="B51">
+        <f>LN(EXP(3))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2">
+      <c r="B52">
+        <f>_xlfn.STDEV.S(B5, B6, B7)</f>
+        <v>4.0414518843273806</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2">
+      <c r="B53">
+        <f>COUNTIF(B18:B21, B18)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2">
+      <c r="B54">
+        <f>IF(B19&gt;B20, 1, 2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2">
+      <c r="B55">
+        <f>IF(B21&gt;B20, 1, 2)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2">
+      <c r="B56">
+        <f>IF(AND(1&lt;2, 3&lt;4), 0, 100)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2">
+      <c r="B57">
+        <f>IF(OR(2&lt;1, 3&lt;4), 0, 100)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2">
+      <c r="B58">
         <f>IF(NOT(2&lt;1), 0, 100)</f>
         <v>0</v>
       </c>
@@ -14050,10 +15158,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{529BA031-6D75-6C46-BAF1-3106D5A9BED1}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView showFormulas="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
@@ -14564,11 +15672,235 @@
         <v>512</v>
       </c>
       <c r="D31" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E31" t="s">
         <v>416</v>
       </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>533</v>
+      </c>
+      <c r="B32" t="s">
+        <v>546</v>
+      </c>
+      <c r="C32" t="s">
+        <v>559</v>
+      </c>
+      <c r="D32" t="s">
+        <v>60</v>
+      </c>
+      <c r="E32" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>534</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>547</v>
+      </c>
+      <c r="C33" t="s">
+        <v>560</v>
+      </c>
+      <c r="D33" t="s">
+        <v>60</v>
+      </c>
+      <c r="E33" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="6" t="s">
+        <v>535</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>548</v>
+      </c>
+      <c r="C34" t="s">
+        <v>561</v>
+      </c>
+      <c r="D34" t="s">
+        <v>60</v>
+      </c>
+      <c r="E34" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>536</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>549</v>
+      </c>
+      <c r="C35" t="s">
+        <v>562</v>
+      </c>
+      <c r="D35" t="s">
+        <v>60</v>
+      </c>
+      <c r="E35" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>537</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>550</v>
+      </c>
+      <c r="C36" t="s">
+        <v>563</v>
+      </c>
+      <c r="D36" t="s">
+        <v>60</v>
+      </c>
+      <c r="E36" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>538</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>551</v>
+      </c>
+      <c r="C37" t="s">
+        <v>564</v>
+      </c>
+      <c r="D37" t="s">
+        <v>60</v>
+      </c>
+      <c r="E37" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>539</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>552</v>
+      </c>
+      <c r="C38" t="s">
+        <v>565</v>
+      </c>
+      <c r="D38" t="s">
+        <v>60</v>
+      </c>
+      <c r="E38" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>540</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>553</v>
+      </c>
+      <c r="C39" t="s">
+        <v>566</v>
+      </c>
+      <c r="D39" t="s">
+        <v>60</v>
+      </c>
+      <c r="E39" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>541</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>554</v>
+      </c>
+      <c r="C40" t="s">
+        <v>567</v>
+      </c>
+      <c r="D40" t="s">
+        <v>60</v>
+      </c>
+      <c r="E40" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="6" t="s">
+        <v>542</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>568</v>
+      </c>
+      <c r="D41" t="s">
+        <v>60</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="6" t="s">
+        <v>543</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>556</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>569</v>
+      </c>
+      <c r="D42" t="s">
+        <v>60</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="6" t="s">
+        <v>544</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>557</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>570</v>
+      </c>
+      <c r="D43" t="s">
+        <v>60</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="6" t="s">
+        <v>545</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>558</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>571</v>
+      </c>
+      <c r="D44" t="s">
+        <v>60</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15075,7 +16407,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71EABA77-C8A8-0247-A6AC-2452B8B329D1}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
@@ -16728,7 +18060,7 @@
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="11" t="s">
         <v>124</v>
       </c>
       <c r="B5">
@@ -16739,7 +18071,7 @@
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="10"/>
+      <c r="A6" s="11"/>
       <c r="B6">
         <v>5</v>
       </c>
@@ -16748,7 +18080,7 @@
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="10"/>
+      <c r="A7" s="11"/>
       <c r="B7">
         <v>10</v>
       </c>
@@ -16757,7 +18089,7 @@
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="10"/>
+      <c r="A8" s="11"/>
       <c r="B8">
         <v>1</v>
       </c>
@@ -16766,7 +18098,7 @@
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="10"/>
+      <c r="A9" s="11"/>
       <c r="B9">
         <v>6</v>
       </c>

</xml_diff>